<commit_message>
Se agrega correcciones y validaciones al proyecto, asimismo se mejoro la base de datos
</commit_message>
<xml_diff>
--- a/src/main/java/Reportes/Cargo.xlsx
+++ b/src/main/java/Reportes/Cargo.xlsx
@@ -12,30 +12,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Sistema de Registro de Ingreso Y Salidas del Terminal Terrestre El Chimbador</t>
   </si>
   <si>
-    <t>Reporte de Cargos</t>
+    <t>Reporte de Pago</t>
   </si>
   <si>
     <t>Código</t>
   </si>
   <si>
-    <t>Cargo</t>
+    <t>Dni</t>
+  </si>
+  <si>
+    <t>Conductor</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
+    <t>Tipo Vehiculo</t>
+  </si>
+  <si>
+    <t>Destino</t>
+  </si>
+  <si>
+    <t>Fecha Pago</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Tipo de Pago</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Administrador</t>
+    <t>75156514</t>
+  </si>
+  <si>
+    <t>Lorenzo Daniel Arteaga Gordillo</t>
+  </si>
+  <si>
+    <t>BXI-IJT</t>
+  </si>
+  <si>
+    <t>Bus de Transporte</t>
+  </si>
+  <si>
+    <t>2023-12-05 03:23:03</t>
+  </si>
+  <si>
+    <t>100.0</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>Vigilante de Garita</t>
+    <t>2023-12-05 03:25:01</t>
+  </si>
+  <si>
+    <t>150.0</t>
   </si>
 </sst>
 </file>
@@ -161,14 +200,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" zoomScale="110"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="7.8984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.05859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="19.72265625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.57421875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.23828125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.43359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -188,21 +230,84 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregaron nuevas vistas al proyecto, para que sea atractivo al cliente
</commit_message>
<xml_diff>
--- a/src/main/java/Reportes/Cargo.xlsx
+++ b/src/main/java/Reportes/Cargo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Sistema de Registro de Ingreso Y Salidas del Terminal Terrestre El Chimbador</t>
   </si>
@@ -47,34 +47,118 @@
     <t>Tipo de Pago</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>75156514</t>
+  </si>
+  <si>
+    <t>Lorenzo Daniel Arteaga Gordillo</t>
+  </si>
+  <si>
+    <t>BXI-IJT</t>
+  </si>
+  <si>
+    <t>Bus de Transporte</t>
+  </si>
+  <si>
+    <t>Áncash - Aija - Coris</t>
+  </si>
+  <si>
+    <t>2023-12-05 09:11:19</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>75156514</t>
-  </si>
-  <si>
-    <t>Lorenzo Daniel Arteaga Gordillo</t>
-  </si>
-  <si>
-    <t>BXI-IJT</t>
-  </si>
-  <si>
-    <t>Bus de Transporte</t>
-  </si>
-  <si>
-    <t>2023-12-05 03:23:03</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2023-12-05 03:25:01</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>98765687</t>
+  </si>
+  <si>
+    <t>isaac iva takamura rojas</t>
+  </si>
+  <si>
+    <t>Amazonas - Luya - Inguilpata</t>
+  </si>
+  <si>
+    <t>2023-12-05 09:27:14</t>
+  </si>
+  <si>
+    <t>900.0</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>B89-PIJ</t>
+  </si>
+  <si>
+    <t>Vehiculo del Personal</t>
+  </si>
+  <si>
+    <t>Áncash - Santa - Santa</t>
+  </si>
+  <si>
+    <t>2023-12-05 14:46:13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Apurímac - Abancay - Abancay</t>
+  </si>
+  <si>
+    <t>2023-12-07 20:14:09</t>
   </si>
   <si>
     <t>150.0</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Amazonas - Chachapoyas - Chachapoyas</t>
+  </si>
+  <si>
+    <t>2023-12-11 07:33:02</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>2023-12-11 07:36:21</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>2023-12-11 07:42:56</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Amazonas - Bongará - Jumbilla</t>
+  </si>
+  <si>
+    <t>2023-12-11 07:44:50</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>2023-12-11 07:47:23</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>2023-12-11 13:21:36</t>
   </si>
 </sst>
 </file>
@@ -167,8 +251,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -186,7 +270,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="11115675"/>
+          <a:ext cx="0" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -200,7 +284,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I9"/>
+  <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" zoomScale="110"/>
   </sheetViews>
@@ -209,8 +293,8 @@
     <col min="1" max="1" width="7.8984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.72265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="24.57421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="6.23828125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.43359375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.2734375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="16.89453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -269,27 +353,27 @@
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -298,16 +382,248 @@
         <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>11</v>
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>